<commit_message>
Added Dictionary for Every Test Case[C
</commit_message>
<xml_diff>
--- a/Resources/TestCasesFile.xlsx
+++ b/Resources/TestCasesFile.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXITS TEST\Flipkart\Flipkart\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DDBA98-267E-4465-A56A-18530374553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47745474-2C6B-4882-B389-44F6709107F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductTestData" sheetId="2" r:id="rId2"/>
+    <sheet name="WishlistTestData" sheetId="3" r:id="rId3"/>
+    <sheet name="AddressTestData" sheetId="4" r:id="rId4"/>
+    <sheet name="LoginTestData" sheetId="5" r:id="rId5"/>
+    <sheet name="HomePageTestData" sheetId="6" r:id="rId6"/>
+    <sheet name="LogoutTestData" sheetId="7" r:id="rId7"/>
+    <sheet name="CartTestData" sheetId="8" r:id="rId8"/>
+    <sheet name="ProductDetailsTestData" sheetId="9" r:id="rId9"/>
+    <sheet name="FlipkartProfileInfoTestData" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -88,33 +96,83 @@
     <t>"12121200120"</t>
   </si>
   <si>
-    <t xml:space="preserve">Exectuiton  </t>
-  </si>
-  <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
-    <t>Add Cart</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Gurugram</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Execution Required</t>
+  </si>
+  <si>
+    <t>relevantProducts</t>
+  </si>
+  <si>
+    <t>sortProductByPriceHtoL</t>
+  </si>
+  <si>
+    <t>sortProductByPriceLtoH</t>
+  </si>
+  <si>
+    <t>chooseProductBrand</t>
+  </si>
+  <si>
+    <t>chooseProductRating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>iphone</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>removeFromwishlist</t>
+  </si>
+  <si>
+    <t>addTowishlist</t>
+  </si>
+  <si>
+    <t>iPhone</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>getProductsInwishlist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,8 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -499,7 +558,7 @@
         <v>14</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -510,41 +569,286 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09FD317-6926-4327-9D66-AB93A9F03E2F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3697BF9-5781-42B5-9705-AC1492885E8B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="24.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506A06CD-C5DC-43C2-8B00-08128CFC24D5}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.54296875" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E92A36-70D1-4083-A71D-8D3EB4343346}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2F33618-83EF-4EDE-8D15-14C910AEAE0E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC1FDB6-6D98-4AAD-84B9-4D68F883C6B7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF64FB4C-3955-42F2-B73E-D390AE6D2314}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0F6099-DB78-4330-8844-85826A4C96A8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCD1F56-7375-4558-A79D-51A307C209BF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>